<commit_message>
added DOI links to all (but one) of papers
</commit_message>
<xml_diff>
--- a/research papers/summary.xlsx
+++ b/research papers/summary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bradl\Desktop\uni\final-project\research papers\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3514273F-E47F-45C7-BD1F-03AF6F9C2E4B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6E241F8-A8CB-4014-8C7C-ECD946E8D1BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{85C2B9D3-E6D8-4805-9C5F-61C1282897A0}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{85C2B9D3-E6D8-4805-9C5F-61C1282897A0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,14 +34,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="89">
   <si>
     <t>Year</t>
   </si>
   <si>
-    <t>Number</t>
-  </si>
-  <si>
     <t>Author(s)</t>
   </si>
   <si>
@@ -51,9 +48,6 @@
     <t>Notes</t>
   </si>
   <si>
-    <t>A COMPARISON OF DEEP LEARNING METHODS FOR ENVIRONMENTAL SOUND</t>
-  </si>
-  <si>
     <t>A Hybrid ANN-LSTM Speaker Identification Using Advanced Feature Extraction Techniques</t>
   </si>
   <si>
@@ -220,16 +214,111 @@
   </si>
   <si>
     <t>Abdulmajeed, N. Q., Al-Khateeb, B. and Mohammed, M. A.</t>
+  </si>
+  <si>
+    <t>Link (DOI)</t>
+  </si>
+  <si>
+    <t>A COMPARISON OF DEEP LEARNING METHODS FOR ENVIRONMENTAL SOUND DETECTION</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.3991/ijim.v18i08.45917</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.24996/ijs.2025.66.5.23</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1007/s11042-023-15891-z</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1145/3618104</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1080/03772063.2023.2252392</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.3390/app142210426</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1111/2041-210X.70148</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1111/exsy.13535</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.32622/ijrat.76201926</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1016/j.ecoinf.2024.102637</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1145/3322240</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1016/j.iswa.2022.200115</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1016/j.patcog.2022.109025</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1007/s10462-025-11106-z</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1109/INDICON56171.2022.10039921</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1080/0952813X.2022.2092560</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.31577/cai_2023_5_1255</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.3390/sci6020021</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1007/s10462-024-11065-x</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.3233/KES-210073</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1109/IS262782.2024.10704131</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.3233/JIFS-232812</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1111/exsy.13327</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.48550/arXiv.1703.06902</t>
+  </si>
+  <si>
+    <t>https://eudoxuspress.com/index.php/pub/article/view/591</t>
+  </si>
+  <si>
+    <t>Have Read?</t>
+  </si>
+  <si>
+    <t>No.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -252,16 +341,19 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -277,10 +369,33 @@
 </styleSheet>
 </file>
 
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{AC1F2967-0024-4A64-83DF-79AEAD2801CB}" name="Table1" displayName="Table1" ref="A2:K27" totalsRowShown="0">
+  <autoFilter ref="A2:K27" xr:uid="{AC1F2967-0024-4A64-83DF-79AEAD2801CB}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:I27">
+    <sortCondition ref="E2:E27"/>
+  </sortState>
+  <tableColumns count="11">
+    <tableColumn id="1" xr3:uid="{2477AE6C-09CD-4E41-9A78-201470F65F68}" name="No."/>
+    <tableColumn id="2" xr3:uid="{2137C14E-709A-44D6-9F25-85BFB2A802FF}" name="Year"/>
+    <tableColumn id="3" xr3:uid="{E6FBECEB-2559-474F-B786-551E53F4B8CF}" name="Link (DOI)"/>
+    <tableColumn id="4" xr3:uid="{642ABAD3-E09C-49A8-9261-613D9B127627}" name="Author(s)"/>
+    <tableColumn id="5" xr3:uid="{94060E6B-2E8D-46A2-ABEC-C27BD7D0571D}" name="Title"/>
+    <tableColumn id="7" xr3:uid="{4A6E70C0-EA6F-4514-A197-53469A2E1B8B}" name="Title relevant?"/>
+    <tableColumn id="8" xr3:uid="{0656883B-7AD5-4D3F-85D1-2408F437A901}" name="Abstract relevant?"/>
+    <tableColumn id="9" xr3:uid="{EDEBB1FF-01CB-4EE5-A91F-81FDDEDD58F4}" name="Content relevant?"/>
+    <tableColumn id="10" xr3:uid="{BCD6016A-4822-4E1A-A929-76A27016C417}" name="Include in dissertation?"/>
+    <tableColumn id="11" xr3:uid="{5CFCAADB-3FE1-4F32-8C8A-D4CD54B6121D}" name="Have Read?"/>
+    <tableColumn id="12" xr3:uid="{ADCB4EF4-4758-4152-8A78-4C69AD16369E}" name="Notes"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -318,7 +433,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -424,7 +539,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -566,7 +681,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -574,415 +689,529 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77C2DB88-371A-4ABD-A87E-357F7B7DC5EB}">
-  <dimension ref="A1:I27"/>
+  <dimension ref="A1:K27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="92.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="136.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="55.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="92.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="136.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="24.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="F1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="G1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="H1" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>1</v>
+        <v>88</v>
       </c>
       <c r="B2" t="s">
         <v>0</v>
       </c>
       <c r="C2" t="s">
+        <v>60</v>
+      </c>
+      <c r="D2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2" t="s">
         <v>2</v>
       </c>
-      <c r="D2" t="s">
+      <c r="F2" t="s">
+        <v>28</v>
+      </c>
+      <c r="G2" t="s">
+        <v>29</v>
+      </c>
+      <c r="H2" t="s">
+        <v>31</v>
+      </c>
+      <c r="I2" t="s">
+        <v>35</v>
+      </c>
+      <c r="J2" t="s">
+        <v>87</v>
+      </c>
+      <c r="K2" t="s">
         <v>3</v>
       </c>
-      <c r="E2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F2" t="s">
-        <v>30</v>
-      </c>
-      <c r="G2" t="s">
-        <v>31</v>
-      </c>
-      <c r="H2" t="s">
-        <v>33</v>
-      </c>
-      <c r="I2" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
       <c r="B3">
         <v>2017</v>
       </c>
-      <c r="C3" t="s">
-        <v>48</v>
+      <c r="C3" s="2" t="s">
+        <v>85</v>
       </c>
       <c r="D3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+        <v>46</v>
+      </c>
+      <c r="E3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2</v>
       </c>
       <c r="B4">
         <v>2025</v>
       </c>
-      <c r="C4" t="s">
-        <v>55</v>
+      <c r="C4" s="2" t="s">
+        <v>63</v>
       </c>
       <c r="D4" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+        <v>53</v>
+      </c>
+      <c r="E4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>3</v>
       </c>
       <c r="B5">
         <v>2024</v>
       </c>
-      <c r="C5" t="s">
-        <v>47</v>
+      <c r="C5" s="2" t="s">
+        <v>62</v>
       </c>
       <c r="D5" t="s">
+        <v>45</v>
+      </c>
+      <c r="E5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>19</v>
+      </c>
+      <c r="B6">
+        <v>2023</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="D6" t="s">
+        <v>36</v>
+      </c>
+      <c r="E6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>20</v>
+      </c>
+      <c r="B7">
+        <v>2023</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="D7" t="s">
+        <v>37</v>
+      </c>
+      <c r="E7" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>4</v>
+      </c>
+      <c r="B8">
+        <v>2024</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="D8" t="s">
+        <v>56</v>
+      </c>
+      <c r="E8" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>5</v>
+      </c>
+      <c r="B9">
+        <v>2024</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="D9" t="s">
+        <v>51</v>
+      </c>
+      <c r="E9" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>4</v>
-      </c>
-      <c r="B6">
-        <v>2024</v>
-      </c>
-      <c r="C6" t="s">
-        <v>58</v>
-      </c>
-      <c r="D6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>5</v>
-      </c>
-      <c r="B7">
-        <v>2024</v>
-      </c>
-      <c r="C7" t="s">
-        <v>53</v>
-      </c>
-      <c r="D7" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10">
         <v>6</v>
-      </c>
-      <c r="B8">
-        <v>2025</v>
-      </c>
-      <c r="C8" t="s">
-        <v>59</v>
-      </c>
-      <c r="D8" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>7</v>
-      </c>
-      <c r="B9">
-        <v>2023</v>
-      </c>
-      <c r="C9" t="s">
-        <v>52</v>
-      </c>
-      <c r="D9" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <v>8</v>
       </c>
       <c r="B10">
         <v>2025</v>
       </c>
-      <c r="C10" t="s">
-        <v>49</v>
+      <c r="C10" s="2" t="s">
+        <v>68</v>
       </c>
       <c r="D10" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+        <v>57</v>
+      </c>
+      <c r="E10" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B11">
         <v>2023</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C11" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="D11" t="s">
+        <v>50</v>
+      </c>
+      <c r="E11" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>18</v>
+      </c>
+      <c r="B12">
+        <v>2019</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="D12" t="s">
+        <v>34</v>
+      </c>
+      <c r="E12" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>16</v>
+      </c>
+      <c r="B13">
+        <v>2019</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="D13" t="s">
+        <v>32</v>
+      </c>
+      <c r="E13" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>23</v>
+      </c>
+      <c r="B14">
+        <v>2022</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="D14" t="s">
+        <v>42</v>
+      </c>
+      <c r="E14" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>17</v>
+      </c>
+      <c r="B15">
+        <v>2022</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="D15" t="s">
+        <v>33</v>
+      </c>
+      <c r="E15" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>8</v>
+      </c>
+      <c r="B16">
+        <v>2025</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="D16" t="s">
+        <v>47</v>
+      </c>
+      <c r="E16" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>21</v>
+      </c>
+      <c r="B17">
+        <v>2022</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="D17" t="s">
+        <v>38</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>9</v>
+      </c>
+      <c r="B18">
+        <v>2023</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="D18" t="s">
+        <v>52</v>
+      </c>
+      <c r="E18" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>10</v>
+      </c>
+      <c r="B19">
+        <v>2023</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="D19" t="s">
+        <v>58</v>
+      </c>
+      <c r="E19" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>11</v>
+      </c>
+      <c r="B20">
+        <v>2024</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="D20" t="s">
+        <v>48</v>
+      </c>
+      <c r="E20" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>24</v>
+      </c>
+      <c r="B21">
+        <v>2024</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="D21" t="s">
+        <v>43</v>
+      </c>
+      <c r="E21" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>12</v>
+      </c>
+      <c r="B22">
+        <v>2024</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="D22" t="s">
         <v>54</v>
       </c>
-      <c r="D11" t="s">
+      <c r="E22" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>22</v>
+      </c>
+      <c r="B23">
+        <v>2024</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="D23" t="s">
+        <v>41</v>
+      </c>
+      <c r="E23" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24">
         <v>13</v>
       </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12">
-        <v>10</v>
-      </c>
-      <c r="B12">
+      <c r="B24">
+        <v>2021</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="D24" t="s">
+        <v>49</v>
+      </c>
+      <c r="E24" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>25</v>
+      </c>
+      <c r="B25">
+        <v>2024</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="D25" t="s">
+        <v>44</v>
+      </c>
+      <c r="E25" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>14</v>
+      </c>
+      <c r="B26">
         <v>2023</v>
       </c>
-      <c r="C12" t="s">
-        <v>60</v>
-      </c>
-      <c r="D12" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13">
-        <v>11</v>
-      </c>
-      <c r="B13">
-        <v>2024</v>
-      </c>
-      <c r="C13" t="s">
-        <v>50</v>
-      </c>
-      <c r="D13" t="s">
+      <c r="C26" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="D26" t="s">
+        <v>55</v>
+      </c>
+      <c r="E26" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27">
         <v>15</v>
       </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14">
-        <v>12</v>
-      </c>
-      <c r="B14">
-        <v>2024</v>
-      </c>
-      <c r="C14" t="s">
-        <v>56</v>
-      </c>
-      <c r="D14" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15">
-        <v>13</v>
-      </c>
-      <c r="B15">
-        <v>2021</v>
-      </c>
-      <c r="C15" t="s">
-        <v>51</v>
-      </c>
-      <c r="D15" t="s">
+      <c r="B27">
+        <v>2023</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="D27" t="s">
+        <v>59</v>
+      </c>
+      <c r="E27" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16">
-        <v>14</v>
-      </c>
-      <c r="B16">
-        <v>2023</v>
-      </c>
-      <c r="C16" t="s">
-        <v>57</v>
-      </c>
-      <c r="D16" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17">
-        <v>15</v>
-      </c>
-      <c r="B17">
-        <v>2023</v>
-      </c>
-      <c r="C17" t="s">
-        <v>61</v>
-      </c>
-      <c r="D17" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18">
-        <v>16</v>
-      </c>
-      <c r="B18">
-        <v>2019</v>
-      </c>
-      <c r="C18" t="s">
-        <v>34</v>
-      </c>
-      <c r="D18" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19">
-        <v>17</v>
-      </c>
-      <c r="B19">
-        <v>2022</v>
-      </c>
-      <c r="C19" t="s">
-        <v>35</v>
-      </c>
-      <c r="D19" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20">
-        <v>18</v>
-      </c>
-      <c r="B20">
-        <v>2019</v>
-      </c>
-      <c r="C20" t="s">
-        <v>36</v>
-      </c>
-      <c r="D20" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21">
-        <v>19</v>
-      </c>
-      <c r="B21">
-        <v>2023</v>
-      </c>
-      <c r="C21" t="s">
-        <v>38</v>
-      </c>
-      <c r="D21" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22">
-        <v>20</v>
-      </c>
-      <c r="B22">
-        <v>2023</v>
-      </c>
-      <c r="C22" t="s">
-        <v>39</v>
-      </c>
-      <c r="D22" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23">
-        <v>21</v>
-      </c>
-      <c r="B23">
-        <v>2022</v>
-      </c>
-      <c r="C23" t="s">
-        <v>40</v>
-      </c>
-      <c r="D23" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24">
-        <v>22</v>
-      </c>
-      <c r="B24">
-        <v>2024</v>
-      </c>
-      <c r="C24" t="s">
-        <v>43</v>
-      </c>
-      <c r="D24" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25">
-        <v>23</v>
-      </c>
-      <c r="B25">
-        <v>2022</v>
-      </c>
-      <c r="C25" t="s">
-        <v>44</v>
-      </c>
-      <c r="D25" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26">
-        <v>24</v>
-      </c>
-      <c r="B26">
-        <v>2024</v>
-      </c>
-      <c r="C26" t="s">
-        <v>45</v>
-      </c>
-      <c r="D26" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27">
-        <v>25</v>
-      </c>
-      <c r="B27">
-        <v>2024</v>
-      </c>
-      <c r="C27" t="s">
-        <v>46</v>
-      </c>
-      <c r="D27" t="s">
-        <v>29</v>
-      </c>
-    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C10" r:id="rId1" xr:uid="{662C990B-B86A-4079-894A-3E3E5E65D958}"/>
+    <hyperlink ref="C11" r:id="rId2" xr:uid="{6C418B6D-6C0C-43CB-9861-B0A9C3405037}"/>
+    <hyperlink ref="C24" r:id="rId3" xr:uid="{687D37D5-6A53-4809-B0D4-39187B9CDB51}"/>
+    <hyperlink ref="C26" r:id="rId4" xr:uid="{76EB6431-BC9E-4F14-A71B-C6B95C564741}"/>
+    <hyperlink ref="C27" r:id="rId5" xr:uid="{ED027085-A4A7-4B84-A093-30D4B8946EC5}"/>
+    <hyperlink ref="C12" r:id="rId6" xr:uid="{DE3AD58A-9EF7-4B73-9497-2A6221CBF2BA}"/>
+    <hyperlink ref="C6" r:id="rId7" xr:uid="{E87626ED-A48A-46C1-B0A1-D92709122E5D}"/>
+    <hyperlink ref="C17" r:id="rId8" xr:uid="{F18B3E29-0693-4E1D-A563-29F1B6D7D473}"/>
+    <hyperlink ref="C23" r:id="rId9" xr:uid="{FBA6D984-389D-4666-AF69-2DF781698029}"/>
+    <hyperlink ref="C25" r:id="rId10" xr:uid="{8419B468-9260-4EC4-B8B1-51A4A07F19E0}"/>
+    <hyperlink ref="C19" r:id="rId11" xr:uid="{7DF0F400-5600-4B7E-B147-67DA86069481}"/>
+    <hyperlink ref="C20" r:id="rId12" xr:uid="{2B967755-ACC4-42EE-98B5-27C84EBAFA42}"/>
+    <hyperlink ref="C22" r:id="rId13" xr:uid="{EE1231E6-9DB3-40E2-94A0-4ABC9DCA02F3}"/>
+    <hyperlink ref="C21" r:id="rId14" xr:uid="{94DF5807-DCFB-44C1-9A14-0E48C9156EC9}"/>
+    <hyperlink ref="C18" r:id="rId15" xr:uid="{FF7FB77C-809F-4107-A972-E7940B05389B}"/>
+    <hyperlink ref="C16" r:id="rId16" xr:uid="{DD854D55-9428-45F9-ACBC-BDC97A21F51F}"/>
+    <hyperlink ref="C15" r:id="rId17" xr:uid="{1F6B8341-332D-49CE-855C-75A637031AFC}"/>
+    <hyperlink ref="C14" r:id="rId18" xr:uid="{3C15B722-4312-44AB-958D-DD3666D004AF}"/>
+    <hyperlink ref="C13" r:id="rId19" xr:uid="{61922079-14BC-47D8-82D1-7B7D9C9DE486}"/>
+    <hyperlink ref="C9" r:id="rId20" xr:uid="{503ADAC8-617F-48DD-8510-1FD61FF7DA22}"/>
+    <hyperlink ref="C8" r:id="rId21" xr:uid="{7001F43B-2968-46DB-AF8B-B7DD2691E5FD}"/>
+    <hyperlink ref="C7" r:id="rId22" xr:uid="{2DE5B6CE-7725-4C17-B5D4-0DFA9BD26432}"/>
+    <hyperlink ref="C5" r:id="rId23" xr:uid="{4944660B-A59A-41C2-9863-55EFDDE038AE}"/>
+    <hyperlink ref="C4" r:id="rId24" xr:uid="{C69B36F0-2B89-47B6-BC31-ACDF79F49B32}"/>
+    <hyperlink ref="C3" r:id="rId25" xr:uid="{03930357-F0F9-462D-A13B-CBD1C1B8C72E}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId26"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added more research papers and notes
</commit_message>
<xml_diff>
--- a/research papers/summary.xlsx
+++ b/research papers/summary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bradl\Desktop\uni\final-project\research papers\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6E241F8-A8CB-4014-8C7C-ECD946E8D1BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{034AFB50-43D4-42D8-8FC6-79F2DDC38B5A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{85C2B9D3-E6D8-4805-9C5F-61C1282897A0}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{85C2B9D3-E6D8-4805-9C5F-61C1282897A0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="114">
   <si>
     <t>Year</t>
   </si>
@@ -66,9 +66,6 @@
     <t>Artificial intelligence for heart sound classification A review</t>
   </si>
   <si>
-    <t>Environmental sound recognition on embedded devices using deep learning a review</t>
-  </si>
-  <si>
     <t>Modified layer deep convolution neural network for text-independent speaker recognition</t>
   </si>
   <si>
@@ -120,9 +117,6 @@
     <t>TinyChirp: Bird Song Recognition Using TinyML Models on Low-power Wireless Acoustic Sensors</t>
   </si>
   <si>
-    <t>Title relevant?</t>
-  </si>
-  <si>
     <t>Abstract relevant?</t>
   </si>
   <si>
@@ -153,9 +147,6 @@
     <t>Choudhary, S., Karthik, C. R., Lakshmi, P. S. and Kumar, S.</t>
   </si>
   <si>
-    <t>Topic</t>
-  </si>
-  <si>
     <t>Rest of paper</t>
   </si>
   <si>
@@ -301,13 +292,130 @@
   </si>
   <si>
     <t>No.</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>Topic, 1 = not relevant at all, 10 = exact topic</t>
+  </si>
+  <si>
+    <t>1 = no deep learning, no audio classification</t>
+  </si>
+  <si>
+    <t>10 = bird song classification w/ deep learning</t>
+  </si>
+  <si>
+    <t>5 = audio classification OR bird/environment sounds</t>
+  </si>
+  <si>
+    <t>Title relevance</t>
+  </si>
+  <si>
+    <t>Environmental sound recognition on embedded devices using deep learning: a review</t>
+  </si>
+  <si>
+    <t>MULTI-LABEL. NOT SINGLE LABEL.
+Mel-frequency spectrograms
+Mel-frequency cepstral coefficient
+Sequential aggregation strategy
+Sigmoid probabilities
+Comparison with transfer learning</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1016/j.apacoust.2014.01.001</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1109/ICASSP.2018.8461814</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1109/ICSCC51209.2021.9528234</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.21437/Interspeech.2018-1705</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1007/s00034-021-01896-2</t>
+  </si>
+  <si>
+    <t>Potamitis, I., Ntalampiras, S., Jahn, O. and Riede, K.</t>
+  </si>
+  <si>
+    <t>Thakur, A., Abrol, V., Sharma, P. and Rajan, P.</t>
+  </si>
+  <si>
+    <t>Noumida, A. and Rajan, R.</t>
+  </si>
+  <si>
+    <t>Rajan, R., Johnson, J. and Kareem, N. A.</t>
+  </si>
+  <si>
+    <t>Automatic Bird Sound Detection in Long Real-Field Recordings: Applications and Tools</t>
+  </si>
+  <si>
+    <t>Deep Learning-Based Automatic Bird Species Identification from Isolated Recordings</t>
+  </si>
+  <si>
+    <t>Compressed Convex Spectral Embedding for Bird Species Classification</t>
+  </si>
+  <si>
+    <t>Deep Convex Representations: Feature Representations for Bioacoustics Classification</t>
+  </si>
+  <si>
+    <t>Bird Call Classification Using DNN-Based Acoustic Modelling</t>
+  </si>
+  <si>
+    <t>Classification of Bird Species using Audio processing and Deep Neural Network.pdf</t>
+  </si>
+  <si>
+    <t>Aggarwal, S. and Sehgal, S.</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1109/ICICICT54557.2022.9917735</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">BE A LESSON ON </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">NOT </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>WHAT TO DO.
+DISGUSTINGLY BAD PAPER.</t>
+    </r>
+  </si>
+  <si>
+    <t>Somewhat</t>
+  </si>
+  <si>
+    <t>Section 3 covers preprocessing
+discrete fourier transform
+mel filterbank
+mel-frequency
+scalogram, spectrogram</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -319,6 +427,14 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -345,18 +461,37 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="5">
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -370,10 +505,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{AC1F2967-0024-4A64-83DF-79AEAD2801CB}" name="Table1" displayName="Table1" ref="A2:K27" totalsRowShown="0">
-  <autoFilter ref="A2:K27" xr:uid="{AC1F2967-0024-4A64-83DF-79AEAD2801CB}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:I27">
-    <sortCondition ref="E2:E27"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{AC1F2967-0024-4A64-83DF-79AEAD2801CB}" name="Table1" displayName="Table1" ref="A5:K36" totalsRowShown="0">
+  <autoFilter ref="A5:K36" xr:uid="{AC1F2967-0024-4A64-83DF-79AEAD2801CB}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A6:K36">
+    <sortCondition descending="1" ref="F5:F36"/>
   </sortState>
   <tableColumns count="11">
     <tableColumn id="1" xr3:uid="{2477AE6C-09CD-4E41-9A78-201470F65F68}" name="No."/>
@@ -381,11 +516,11 @@
     <tableColumn id="3" xr3:uid="{E6FBECEB-2559-474F-B786-551E53F4B8CF}" name="Link (DOI)"/>
     <tableColumn id="4" xr3:uid="{642ABAD3-E09C-49A8-9261-613D9B127627}" name="Author(s)"/>
     <tableColumn id="5" xr3:uid="{94060E6B-2E8D-46A2-ABEC-C27BD7D0571D}" name="Title"/>
-    <tableColumn id="7" xr3:uid="{4A6E70C0-EA6F-4514-A197-53469A2E1B8B}" name="Title relevant?"/>
-    <tableColumn id="8" xr3:uid="{0656883B-7AD5-4D3F-85D1-2408F437A901}" name="Abstract relevant?"/>
-    <tableColumn id="9" xr3:uid="{EDEBB1FF-01CB-4EE5-A91F-81FDDEDD58F4}" name="Content relevant?"/>
-    <tableColumn id="10" xr3:uid="{BCD6016A-4822-4E1A-A929-76A27016C417}" name="Include in dissertation?"/>
-    <tableColumn id="11" xr3:uid="{5CFCAADB-3FE1-4F32-8C8A-D4CD54B6121D}" name="Have Read?"/>
+    <tableColumn id="7" xr3:uid="{4A6E70C0-EA6F-4514-A197-53469A2E1B8B}" name="Title relevance" dataDxfId="4"/>
+    <tableColumn id="8" xr3:uid="{0656883B-7AD5-4D3F-85D1-2408F437A901}" name="Abstract relevant?" dataDxfId="3"/>
+    <tableColumn id="9" xr3:uid="{EDEBB1FF-01CB-4EE5-A91F-81FDDEDD58F4}" name="Content relevant?" dataDxfId="2"/>
+    <tableColumn id="10" xr3:uid="{BCD6016A-4822-4E1A-A929-76A27016C417}" name="Include in dissertation?" dataDxfId="1"/>
+    <tableColumn id="11" xr3:uid="{5CFCAADB-3FE1-4F32-8C8A-D4CD54B6121D}" name="Have Read?" dataDxfId="0"/>
     <tableColumn id="12" xr3:uid="{ADCB4EF4-4758-4152-8A78-4C69AD16369E}" name="Notes"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -393,9 +528,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2013 - 2022">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -433,7 +568,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2013 - 2022">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -539,7 +674,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2013 - 2022">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -681,7 +816,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -689,10 +824,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77C2DB88-371A-4ABD-A87E-357F7B7DC5EB}">
-  <dimension ref="A1:K27"/>
+  <dimension ref="A1:K36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -700,179 +835,182 @@
     <col min="1" max="1" width="6.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="7.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="55.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="92.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23" customWidth="1"/>
     <col min="5" max="5" width="136.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.85546875" customWidth="1"/>
     <col min="7" max="7" width="19.7109375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="19.5703125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="24.42578125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="32.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="F1" t="s">
-        <v>39</v>
-      </c>
-      <c r="G1" t="s">
-        <v>30</v>
-      </c>
-      <c r="H1" t="s">
-        <v>40</v>
+        <v>88</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>88</v>
-      </c>
-      <c r="B2" t="s">
+      <c r="F2" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="F3" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="F4" t="s">
+        <v>87</v>
+      </c>
+      <c r="G4" t="s">
+        <v>28</v>
+      </c>
+      <c r="H4" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>85</v>
+      </c>
+      <c r="B5" t="s">
         <v>0</v>
       </c>
-      <c r="C2" t="s">
-        <v>60</v>
-      </c>
-      <c r="D2" t="s">
+      <c r="C5" t="s">
+        <v>57</v>
+      </c>
+      <c r="D5" t="s">
         <v>1</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E5" t="s">
         <v>2</v>
       </c>
-      <c r="F2" t="s">
-        <v>28</v>
-      </c>
-      <c r="G2" t="s">
+      <c r="F5" t="s">
+        <v>91</v>
+      </c>
+      <c r="G5" t="s">
+        <v>27</v>
+      </c>
+      <c r="H5" t="s">
         <v>29</v>
       </c>
-      <c r="H2" t="s">
-        <v>31</v>
-      </c>
-      <c r="I2" t="s">
-        <v>35</v>
-      </c>
-      <c r="J2" t="s">
-        <v>87</v>
-      </c>
-      <c r="K2" t="s">
+      <c r="I5" t="s">
+        <v>33</v>
+      </c>
+      <c r="J5" t="s">
+        <v>84</v>
+      </c>
+      <c r="K5" t="s">
         <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>1</v>
-      </c>
-      <c r="B3">
-        <v>2017</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="D3" t="s">
-        <v>46</v>
-      </c>
-      <c r="E3" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>2</v>
-      </c>
-      <c r="B4">
-        <v>2025</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="D4" t="s">
-        <v>53</v>
-      </c>
-      <c r="E4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>3</v>
-      </c>
-      <c r="B5">
-        <v>2024</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="D5" t="s">
-        <v>45</v>
-      </c>
-      <c r="E5" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="B6">
-        <v>2023</v>
+        <v>2024</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="D6" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="E6" t="s">
-        <v>21</v>
-      </c>
+        <v>23</v>
+      </c>
+      <c r="F6" s="3">
+        <v>10</v>
+      </c>
+      <c r="G6" s="3"/>
+      <c r="H6" s="3"/>
+      <c r="I6" s="3"/>
+      <c r="J6" s="3"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="B7">
-        <v>2023</v>
+        <v>2024</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>65</v>
+        <v>79</v>
       </c>
       <c r="D7" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="E7" t="s">
-        <v>22</v>
-      </c>
+        <v>26</v>
+      </c>
+      <c r="F7" s="3">
+        <v>10</v>
+      </c>
+      <c r="G7" s="3"/>
+      <c r="H7" s="3"/>
+      <c r="I7" s="3"/>
+      <c r="J7" s="3"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>4</v>
+        <v>28</v>
       </c>
       <c r="B8">
-        <v>2024</v>
+        <v>2021</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>66</v>
+        <v>96</v>
       </c>
       <c r="D8" t="s">
-        <v>56</v>
+        <v>101</v>
       </c>
       <c r="E8" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+        <v>104</v>
+      </c>
+      <c r="F8" s="3">
+        <v>10</v>
+      </c>
+      <c r="G8" s="3"/>
+      <c r="H8" s="3"/>
+      <c r="I8" s="3"/>
+      <c r="J8" s="3"/>
+    </row>
+    <row r="9" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>5</v>
+        <v>31</v>
       </c>
       <c r="B9">
-        <v>2024</v>
+        <v>2022</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>67</v>
+        <v>110</v>
       </c>
       <c r="D9" t="s">
-        <v>51</v>
+        <v>109</v>
       </c>
       <c r="E9" t="s">
-        <v>7</v>
+        <v>108</v>
+      </c>
+      <c r="F9" s="3">
+        <v>10</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="H9" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="I9" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="J9" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="K9" s="1" t="s">
+        <v>111</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
@@ -883,169 +1021,250 @@
         <v>2025</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="D10" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="E10" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="F10" s="3">
+        <v>9</v>
+      </c>
+      <c r="G10" s="3"/>
+      <c r="H10" s="3"/>
+      <c r="I10" s="3"/>
+      <c r="J10" s="3"/>
+    </row>
+    <row r="11" spans="1:11" ht="90" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="B11">
         <v>2023</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>69</v>
+        <v>75</v>
       </c>
       <c r="D11" t="s">
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="E11" t="s">
+        <v>11</v>
+      </c>
+      <c r="F11" s="3">
         <v>9</v>
+      </c>
+      <c r="G11" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="H11" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="I11" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="J11" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="K11" s="1" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B12">
-        <v>2019</v>
+        <v>2023</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
       <c r="D12" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E12" t="s">
-        <v>20</v>
-      </c>
+        <v>21</v>
+      </c>
+      <c r="F12" s="3">
+        <v>9</v>
+      </c>
+      <c r="G12" s="3"/>
+      <c r="H12" s="3"/>
+      <c r="I12" s="3"/>
+      <c r="J12" s="3"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13">
-        <v>16</v>
+        <v>26</v>
       </c>
       <c r="B13">
-        <v>2019</v>
+        <v>2014</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>72</v>
+        <v>94</v>
       </c>
       <c r="D13" t="s">
-        <v>32</v>
+        <v>99</v>
       </c>
       <c r="E13" t="s">
-        <v>18</v>
-      </c>
+        <v>103</v>
+      </c>
+      <c r="F13" s="3">
+        <v>9</v>
+      </c>
+      <c r="G13" s="3"/>
+      <c r="H13" s="3"/>
+      <c r="I13" s="3"/>
+      <c r="J13" s="3"/>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="B14">
-        <v>2022</v>
+        <v>2018</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>74</v>
+        <v>95</v>
       </c>
       <c r="D14" t="s">
-        <v>42</v>
+        <v>100</v>
       </c>
       <c r="E14" t="s">
-        <v>25</v>
-      </c>
+        <v>105</v>
+      </c>
+      <c r="F14" s="3">
+        <v>8</v>
+      </c>
+      <c r="G14" s="3"/>
+      <c r="H14" s="3"/>
+      <c r="I14" s="3"/>
+      <c r="J14" s="3"/>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15">
-        <v>17</v>
+        <v>29</v>
       </c>
       <c r="B15">
-        <v>2022</v>
+        <v>2018</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>73</v>
+        <v>97</v>
       </c>
       <c r="D15" t="s">
-        <v>33</v>
+        <v>100</v>
       </c>
       <c r="E15" t="s">
-        <v>19</v>
-      </c>
+        <v>106</v>
+      </c>
+      <c r="F15" s="3">
+        <v>8</v>
+      </c>
+      <c r="G15" s="3"/>
+      <c r="H15" s="3"/>
+      <c r="I15" s="3"/>
+      <c r="J15" s="3"/>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16">
+        <v>30</v>
+      </c>
+      <c r="B16">
+        <v>2022</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="D16" t="s">
+        <v>102</v>
+      </c>
+      <c r="E16" t="s">
+        <v>107</v>
+      </c>
+      <c r="F16" s="3">
         <v>8</v>
       </c>
-      <c r="B16">
+      <c r="G16" s="3"/>
+      <c r="H16" s="3"/>
+      <c r="I16" s="3"/>
+      <c r="J16" s="3"/>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>1</v>
+      </c>
+      <c r="B17">
+        <v>2017</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="D17" t="s">
+        <v>43</v>
+      </c>
+      <c r="E17" t="s">
+        <v>58</v>
+      </c>
+      <c r="F17" s="3">
+        <v>7</v>
+      </c>
+      <c r="G17" s="3"/>
+      <c r="H17" s="3"/>
+      <c r="I17" s="3"/>
+      <c r="J17" s="3"/>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>3</v>
+      </c>
+      <c r="B18">
+        <v>2024</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="D18" t="s">
+        <v>42</v>
+      </c>
+      <c r="E18" t="s">
+        <v>5</v>
+      </c>
+      <c r="F18" s="3">
+        <v>7</v>
+      </c>
+      <c r="G18" s="3"/>
+      <c r="H18" s="3"/>
+      <c r="I18" s="3"/>
+      <c r="J18" s="3"/>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>8</v>
+      </c>
+      <c r="B19">
         <v>2025</v>
       </c>
-      <c r="C16" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="D16" t="s">
-        <v>47</v>
-      </c>
-      <c r="E16" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17">
-        <v>21</v>
-      </c>
-      <c r="B17">
-        <v>2022</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="D17" t="s">
-        <v>38</v>
-      </c>
-      <c r="E17" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18">
-        <v>9</v>
-      </c>
-      <c r="B18">
-        <v>2023</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="D18" t="s">
-        <v>52</v>
-      </c>
-      <c r="E18" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19">
-        <v>10</v>
-      </c>
-      <c r="B19">
-        <v>2023</v>
-      </c>
       <c r="C19" s="2" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="D19" t="s">
-        <v>58</v>
+        <v>44</v>
       </c>
       <c r="E19" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+        <v>92</v>
+      </c>
+      <c r="F19" s="3">
+        <v>7</v>
+      </c>
+      <c r="G19" s="3"/>
+      <c r="H19" s="3"/>
+      <c r="I19" s="3"/>
+      <c r="J19" s="3"/>
+    </row>
+    <row r="20" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>11</v>
       </c>
@@ -1053,165 +1272,454 @@
         <v>2024</v>
       </c>
       <c r="C20" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="D20" t="s">
+        <v>45</v>
+      </c>
+      <c r="E20" t="s">
+        <v>12</v>
+      </c>
+      <c r="F20" s="3">
+        <v>7</v>
+      </c>
+      <c r="G20" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="D20" t="s">
-        <v>48</v>
-      </c>
-      <c r="E20" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="H20" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="I20" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="J20" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="K20" s="1" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="B21">
-        <v>2024</v>
+        <v>2022</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>79</v>
+        <v>70</v>
       </c>
       <c r="D21" t="s">
-        <v>43</v>
+        <v>31</v>
       </c>
       <c r="E21" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+      <c r="F21" s="3">
+        <v>7</v>
+      </c>
+      <c r="G21" s="3"/>
+      <c r="H21" s="3"/>
+      <c r="I21" s="3"/>
+      <c r="J21" s="3"/>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="B22">
-        <v>2024</v>
+        <v>2019</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>80</v>
+        <v>67</v>
       </c>
       <c r="D22" t="s">
-        <v>54</v>
+        <v>32</v>
       </c>
       <c r="E22" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+      <c r="F22" s="3">
+        <v>7</v>
+      </c>
+      <c r="G22" s="3"/>
+      <c r="H22" s="3"/>
+      <c r="I22" s="3"/>
+      <c r="J22" s="3"/>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B23">
-        <v>2024</v>
+        <v>2022</v>
       </c>
       <c r="C23" s="2" t="s">
         <v>71</v>
       </c>
       <c r="D23" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E23" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F23" s="3">
+        <v>7</v>
+      </c>
+      <c r="G23" s="3"/>
+      <c r="H23" s="3"/>
+      <c r="I23" s="3"/>
+      <c r="J23" s="3"/>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24">
+        <v>5</v>
+      </c>
+      <c r="B24">
+        <v>2024</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="D24" t="s">
+        <v>48</v>
+      </c>
+      <c r="E24" t="s">
+        <v>7</v>
+      </c>
+      <c r="F24" s="3">
+        <v>6</v>
+      </c>
+      <c r="G24" s="3"/>
+      <c r="H24" s="3"/>
+      <c r="I24" s="3"/>
+      <c r="J24" s="3"/>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A25">
         <v>13</v>
       </c>
-      <c r="B24">
+      <c r="B25">
         <v>2021</v>
       </c>
-      <c r="C24" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="D24" t="s">
-        <v>49</v>
-      </c>
-      <c r="E24" t="s">
+      <c r="C25" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="D25" t="s">
+        <v>46</v>
+      </c>
+      <c r="E25" t="s">
+        <v>14</v>
+      </c>
+      <c r="F25" s="3">
+        <v>6</v>
+      </c>
+      <c r="G25" s="3"/>
+      <c r="H25" s="3"/>
+      <c r="I25" s="3"/>
+      <c r="J25" s="3"/>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A26">
         <v>15</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25">
-        <v>25</v>
-      </c>
-      <c r="B25">
-        <v>2024</v>
-      </c>
-      <c r="C25" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="D25" t="s">
-        <v>44</v>
-      </c>
-      <c r="E25" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26">
-        <v>14</v>
       </c>
       <c r="B26">
         <v>2023</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D26" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="E26" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F26" s="3">
+        <v>6</v>
+      </c>
+      <c r="G26" s="3"/>
+      <c r="H26" s="3"/>
+      <c r="I26" s="3"/>
+      <c r="J26" s="3"/>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="B27">
         <v>2023</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>84</v>
+        <v>61</v>
       </c>
       <c r="D27" t="s">
-        <v>59</v>
+        <v>34</v>
       </c>
       <c r="E27" t="s">
+        <v>20</v>
+      </c>
+      <c r="F27" s="3">
+        <v>6</v>
+      </c>
+      <c r="G27" s="3"/>
+      <c r="H27" s="3"/>
+      <c r="I27" s="3"/>
+      <c r="J27" s="3"/>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>21</v>
+      </c>
+      <c r="B28">
+        <v>2022</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="D28" t="s">
+        <v>36</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F28" s="3">
+        <v>6</v>
+      </c>
+      <c r="G28" s="3"/>
+      <c r="H28" s="3"/>
+      <c r="I28" s="3"/>
+      <c r="J28" s="3"/>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>2</v>
+      </c>
+      <c r="B29">
+        <v>2025</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="D29" t="s">
+        <v>50</v>
+      </c>
+      <c r="E29" t="s">
+        <v>4</v>
+      </c>
+      <c r="F29" s="3">
+        <v>5</v>
+      </c>
+      <c r="G29" s="3"/>
+      <c r="H29" s="3"/>
+      <c r="I29" s="3"/>
+      <c r="J29" s="3"/>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>7</v>
+      </c>
+      <c r="B30">
+        <v>2023</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="D30" t="s">
+        <v>47</v>
+      </c>
+      <c r="E30" t="s">
+        <v>9</v>
+      </c>
+      <c r="F30" s="3">
+        <v>5</v>
+      </c>
+      <c r="G30" s="3"/>
+      <c r="H30" s="3"/>
+      <c r="I30" s="3"/>
+      <c r="J30" s="3"/>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>9</v>
+      </c>
+      <c r="B31">
+        <v>2023</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="D31" t="s">
+        <v>49</v>
+      </c>
+      <c r="E31" t="s">
+        <v>10</v>
+      </c>
+      <c r="F31" s="3">
+        <v>5</v>
+      </c>
+      <c r="G31" s="3"/>
+      <c r="H31" s="3"/>
+      <c r="I31" s="3"/>
+      <c r="J31" s="3"/>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>12</v>
+      </c>
+      <c r="B32">
+        <v>2024</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="D32" t="s">
+        <v>51</v>
+      </c>
+      <c r="E32" t="s">
+        <v>13</v>
+      </c>
+      <c r="F32" s="3">
+        <v>5</v>
+      </c>
+      <c r="G32" s="3"/>
+      <c r="H32" s="3"/>
+      <c r="I32" s="3"/>
+      <c r="J32" s="3"/>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>16</v>
+      </c>
+      <c r="B33">
+        <v>2019</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="D33" t="s">
+        <v>30</v>
+      </c>
+      <c r="E33" t="s">
         <v>17</v>
       </c>
+      <c r="F33" s="3">
+        <v>5</v>
+      </c>
+      <c r="G33" s="3"/>
+      <c r="H33" s="3"/>
+      <c r="I33" s="3"/>
+      <c r="J33" s="3"/>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>24</v>
+      </c>
+      <c r="B34">
+        <v>2024</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="D34" t="s">
+        <v>40</v>
+      </c>
+      <c r="E34" t="s">
+        <v>25</v>
+      </c>
+      <c r="F34" s="3">
+        <v>5</v>
+      </c>
+      <c r="G34" s="3"/>
+      <c r="H34" s="3"/>
+      <c r="I34" s="3"/>
+      <c r="J34" s="3"/>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>14</v>
+      </c>
+      <c r="B35">
+        <v>2023</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="D35" t="s">
+        <v>52</v>
+      </c>
+      <c r="E35" t="s">
+        <v>15</v>
+      </c>
+      <c r="F35" s="3">
+        <v>4</v>
+      </c>
+      <c r="G35" s="3"/>
+      <c r="H35" s="3"/>
+      <c r="I35" s="3"/>
+      <c r="J35" s="3"/>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>4</v>
+      </c>
+      <c r="B36">
+        <v>2024</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="D36" t="s">
+        <v>53</v>
+      </c>
+      <c r="E36" t="s">
+        <v>6</v>
+      </c>
+      <c r="F36" s="3">
+        <v>3</v>
+      </c>
+      <c r="G36" s="3"/>
+      <c r="H36" s="3"/>
+      <c r="I36" s="3"/>
+      <c r="J36" s="3"/>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="C10" r:id="rId1" xr:uid="{662C990B-B86A-4079-894A-3E3E5E65D958}"/>
-    <hyperlink ref="C11" r:id="rId2" xr:uid="{6C418B6D-6C0C-43CB-9861-B0A9C3405037}"/>
-    <hyperlink ref="C24" r:id="rId3" xr:uid="{687D37D5-6A53-4809-B0D4-39187B9CDB51}"/>
-    <hyperlink ref="C26" r:id="rId4" xr:uid="{76EB6431-BC9E-4F14-A71B-C6B95C564741}"/>
-    <hyperlink ref="C27" r:id="rId5" xr:uid="{ED027085-A4A7-4B84-A093-30D4B8946EC5}"/>
-    <hyperlink ref="C12" r:id="rId6" xr:uid="{DE3AD58A-9EF7-4B73-9497-2A6221CBF2BA}"/>
-    <hyperlink ref="C6" r:id="rId7" xr:uid="{E87626ED-A48A-46C1-B0A1-D92709122E5D}"/>
-    <hyperlink ref="C17" r:id="rId8" xr:uid="{F18B3E29-0693-4E1D-A563-29F1B6D7D473}"/>
-    <hyperlink ref="C23" r:id="rId9" xr:uid="{FBA6D984-389D-4666-AF69-2DF781698029}"/>
-    <hyperlink ref="C25" r:id="rId10" xr:uid="{8419B468-9260-4EC4-B8B1-51A4A07F19E0}"/>
-    <hyperlink ref="C19" r:id="rId11" xr:uid="{7DF0F400-5600-4B7E-B147-67DA86069481}"/>
+    <hyperlink ref="C30" r:id="rId2" xr:uid="{6C418B6D-6C0C-43CB-9861-B0A9C3405037}"/>
+    <hyperlink ref="C25" r:id="rId3" xr:uid="{687D37D5-6A53-4809-B0D4-39187B9CDB51}"/>
+    <hyperlink ref="C35" r:id="rId4" xr:uid="{76EB6431-BC9E-4F14-A71B-C6B95C564741}"/>
+    <hyperlink ref="C26" r:id="rId5" xr:uid="{ED027085-A4A7-4B84-A093-30D4B8946EC5}"/>
+    <hyperlink ref="C22" r:id="rId6" xr:uid="{DE3AD58A-9EF7-4B73-9497-2A6221CBF2BA}"/>
+    <hyperlink ref="C27" r:id="rId7" xr:uid="{E87626ED-A48A-46C1-B0A1-D92709122E5D}"/>
+    <hyperlink ref="C28" r:id="rId8" xr:uid="{F18B3E29-0693-4E1D-A563-29F1B6D7D473}"/>
+    <hyperlink ref="C6" r:id="rId9" xr:uid="{FBA6D984-389D-4666-AF69-2DF781698029}"/>
+    <hyperlink ref="C7" r:id="rId10" xr:uid="{8419B468-9260-4EC4-B8B1-51A4A07F19E0}"/>
+    <hyperlink ref="C11" r:id="rId11" xr:uid="{7DF0F400-5600-4B7E-B147-67DA86069481}"/>
     <hyperlink ref="C20" r:id="rId12" xr:uid="{2B967755-ACC4-42EE-98B5-27C84EBAFA42}"/>
-    <hyperlink ref="C22" r:id="rId13" xr:uid="{EE1231E6-9DB3-40E2-94A0-4ABC9DCA02F3}"/>
-    <hyperlink ref="C21" r:id="rId14" xr:uid="{94DF5807-DCFB-44C1-9A14-0E48C9156EC9}"/>
-    <hyperlink ref="C18" r:id="rId15" xr:uid="{FF7FB77C-809F-4107-A972-E7940B05389B}"/>
-    <hyperlink ref="C16" r:id="rId16" xr:uid="{DD854D55-9428-45F9-ACBC-BDC97A21F51F}"/>
-    <hyperlink ref="C15" r:id="rId17" xr:uid="{1F6B8341-332D-49CE-855C-75A637031AFC}"/>
-    <hyperlink ref="C14" r:id="rId18" xr:uid="{3C15B722-4312-44AB-958D-DD3666D004AF}"/>
-    <hyperlink ref="C13" r:id="rId19" xr:uid="{61922079-14BC-47D8-82D1-7B7D9C9DE486}"/>
-    <hyperlink ref="C9" r:id="rId20" xr:uid="{503ADAC8-617F-48DD-8510-1FD61FF7DA22}"/>
-    <hyperlink ref="C8" r:id="rId21" xr:uid="{7001F43B-2968-46DB-AF8B-B7DD2691E5FD}"/>
-    <hyperlink ref="C7" r:id="rId22" xr:uid="{2DE5B6CE-7725-4C17-B5D4-0DFA9BD26432}"/>
-    <hyperlink ref="C5" r:id="rId23" xr:uid="{4944660B-A59A-41C2-9863-55EFDDE038AE}"/>
-    <hyperlink ref="C4" r:id="rId24" xr:uid="{C69B36F0-2B89-47B6-BC31-ACDF79F49B32}"/>
-    <hyperlink ref="C3" r:id="rId25" xr:uid="{03930357-F0F9-462D-A13B-CBD1C1B8C72E}"/>
+    <hyperlink ref="C32" r:id="rId13" xr:uid="{EE1231E6-9DB3-40E2-94A0-4ABC9DCA02F3}"/>
+    <hyperlink ref="C34" r:id="rId14" xr:uid="{94DF5807-DCFB-44C1-9A14-0E48C9156EC9}"/>
+    <hyperlink ref="C31" r:id="rId15" xr:uid="{FF7FB77C-809F-4107-A972-E7940B05389B}"/>
+    <hyperlink ref="C19" r:id="rId16" xr:uid="{DD854D55-9428-45F9-ACBC-BDC97A21F51F}"/>
+    <hyperlink ref="C21" r:id="rId17" xr:uid="{1F6B8341-332D-49CE-855C-75A637031AFC}"/>
+    <hyperlink ref="C23" r:id="rId18" xr:uid="{3C15B722-4312-44AB-958D-DD3666D004AF}"/>
+    <hyperlink ref="C33" r:id="rId19" xr:uid="{61922079-14BC-47D8-82D1-7B7D9C9DE486}"/>
+    <hyperlink ref="C24" r:id="rId20" xr:uid="{503ADAC8-617F-48DD-8510-1FD61FF7DA22}"/>
+    <hyperlink ref="C36" r:id="rId21" xr:uid="{7001F43B-2968-46DB-AF8B-B7DD2691E5FD}"/>
+    <hyperlink ref="C12" r:id="rId22" xr:uid="{2DE5B6CE-7725-4C17-B5D4-0DFA9BD26432}"/>
+    <hyperlink ref="C18" r:id="rId23" xr:uid="{4944660B-A59A-41C2-9863-55EFDDE038AE}"/>
+    <hyperlink ref="C29" r:id="rId24" xr:uid="{C69B36F0-2B89-47B6-BC31-ACDF79F49B32}"/>
+    <hyperlink ref="C17" r:id="rId25" xr:uid="{03930357-F0F9-462D-A13B-CBD1C1B8C72E}"/>
+    <hyperlink ref="C13" r:id="rId26" xr:uid="{95A1E5A0-980E-4DB3-8046-566D2E946C8C}"/>
+    <hyperlink ref="C14" r:id="rId27" xr:uid="{7819739D-ADAC-426C-BC29-1A3209D63F34}"/>
+    <hyperlink ref="C8" r:id="rId28" xr:uid="{2D1D63DF-CA4E-4BC1-9C5C-6AF3A4C0CE05}"/>
+    <hyperlink ref="C15" r:id="rId29" xr:uid="{90402084-E9E4-4A3D-A1CA-D4B73CBB3CDE}"/>
+    <hyperlink ref="C16" r:id="rId30" xr:uid="{CB934A96-3CB2-4775-A540-BA09DC06EED6}"/>
+    <hyperlink ref="C9" r:id="rId31" xr:uid="{9E20CD7C-6E43-408A-93EB-504D56252D0E}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
-    <tablePart r:id="rId26"/>
+    <tablePart r:id="rId32"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
modified research paper folder
</commit_message>
<xml_diff>
--- a/research papers/summary.xlsx
+++ b/research papers/summary.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bradl\Desktop\uni\final-project\research papers\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{034AFB50-43D4-42D8-8FC6-79F2DDC38B5A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{670AB422-E59F-47F1-8E04-5C1D2658E383}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{85C2B9D3-E6D8-4805-9C5F-61C1282897A0}"/>
+    <workbookView xWindow="-28920" yWindow="5280" windowWidth="29040" windowHeight="15840" xr2:uid="{85C2B9D3-E6D8-4805-9C5F-61C1282897A0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="115">
   <si>
     <t>Year</t>
   </si>
@@ -133,9 +133,6 @@
   </si>
   <si>
     <t>Mohammad, A. and Tripathi, M. M.</t>
-  </si>
-  <si>
-    <t>Include in dissertation?</t>
   </si>
   <si>
     <t>Prashanth, A., Jayalakshmi, S. L. and Vedhapriyavadhana, R.</t>
@@ -409,6 +406,12 @@
 mel filterbank
 mel-frequency
 scalogram, spectrogram</t>
+  </si>
+  <si>
+    <t>Included in dissertation?</t>
+  </si>
+  <si>
+    <t>Mangalam Sankupellay and Dmitry Konovalov</t>
   </si>
 </sst>
 </file>
@@ -505,10 +508,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{AC1F2967-0024-4A64-83DF-79AEAD2801CB}" name="Table1" displayName="Table1" ref="A5:K36" totalsRowShown="0">
-  <autoFilter ref="A5:K36" xr:uid="{AC1F2967-0024-4A64-83DF-79AEAD2801CB}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{AC1F2967-0024-4A64-83DF-79AEAD2801CB}" name="Table1" displayName="Table1" ref="A5:K37" totalsRowShown="0">
+  <autoFilter ref="A5:K37" xr:uid="{AC1F2967-0024-4A64-83DF-79AEAD2801CB}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A6:K36">
-    <sortCondition descending="1" ref="F5:F36"/>
+    <sortCondition ref="E5:E36"/>
   </sortState>
   <tableColumns count="11">
     <tableColumn id="1" xr3:uid="{2477AE6C-09CD-4E41-9A78-201470F65F68}" name="No."/>
@@ -519,7 +522,7 @@
     <tableColumn id="7" xr3:uid="{4A6E70C0-EA6F-4514-A197-53469A2E1B8B}" name="Title relevance" dataDxfId="4"/>
     <tableColumn id="8" xr3:uid="{0656883B-7AD5-4D3F-85D1-2408F437A901}" name="Abstract relevant?" dataDxfId="3"/>
     <tableColumn id="9" xr3:uid="{EDEBB1FF-01CB-4EE5-A91F-81FDDEDD58F4}" name="Content relevant?" dataDxfId="2"/>
-    <tableColumn id="10" xr3:uid="{BCD6016A-4822-4E1A-A929-76A27016C417}" name="Include in dissertation?" dataDxfId="1"/>
+    <tableColumn id="10" xr3:uid="{BCD6016A-4822-4E1A-A929-76A27016C417}" name="Included in dissertation?" dataDxfId="1"/>
     <tableColumn id="11" xr3:uid="{5CFCAADB-3FE1-4F32-8C8A-D4CD54B6121D}" name="Have Read?" dataDxfId="0"/>
     <tableColumn id="12" xr3:uid="{ADCB4EF4-4758-4152-8A78-4C69AD16369E}" name="Notes"/>
   </tableColumns>
@@ -824,62 +827,62 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77C2DB88-371A-4ABD-A87E-357F7B7DC5EB}">
-  <dimension ref="A1:K36"/>
+  <dimension ref="A1:K37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="6.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="7.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="55.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="23" customWidth="1"/>
-    <col min="5" max="5" width="136.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.42578125" customWidth="1"/>
+    <col min="4" max="4" width="92.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="25" customWidth="1"/>
     <col min="6" max="6" width="16.85546875" customWidth="1"/>
     <col min="7" max="7" width="19.7109375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="24.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="25.5703125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="13.5703125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="32.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="F1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="F2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="F3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="F4" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="G4" t="s">
         <v>28</v>
       </c>
       <c r="H4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B5" t="s">
         <v>0</v>
       </c>
       <c r="C5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D5" t="s">
         <v>1</v>
@@ -888,7 +891,7 @@
         <v>2</v>
       </c>
       <c r="F5" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="G5" t="s">
         <v>27</v>
@@ -897,10 +900,10 @@
         <v>29</v>
       </c>
       <c r="I5" t="s">
-        <v>33</v>
+        <v>113</v>
       </c>
       <c r="J5" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="K5" t="s">
         <v>3</v>
@@ -908,22 +911,22 @@
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>22</v>
+        <v>1</v>
       </c>
       <c r="B6">
-        <v>2024</v>
+        <v>2017</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>68</v>
+        <v>81</v>
       </c>
       <c r="D6" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="E6" t="s">
-        <v>23</v>
+        <v>57</v>
       </c>
       <c r="F6" s="3">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="G6" s="3"/>
       <c r="H6" s="3"/>
@@ -932,22 +935,22 @@
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>25</v>
+        <v>2</v>
       </c>
       <c r="B7">
-        <v>2024</v>
+        <v>2025</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>79</v>
+        <v>59</v>
       </c>
       <c r="D7" t="s">
-        <v>41</v>
+        <v>49</v>
       </c>
       <c r="E7" t="s">
-        <v>26</v>
+        <v>4</v>
       </c>
       <c r="F7" s="3">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="G7" s="3"/>
       <c r="H7" s="3"/>
@@ -956,78 +959,67 @@
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>28</v>
+        <v>3</v>
       </c>
       <c r="B8">
-        <v>2021</v>
+        <v>2024</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>96</v>
+        <v>58</v>
       </c>
       <c r="D8" t="s">
-        <v>101</v>
+        <v>41</v>
       </c>
       <c r="E8" t="s">
-        <v>104</v>
+        <v>5</v>
       </c>
       <c r="F8" s="3">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="G8" s="3"/>
       <c r="H8" s="3"/>
       <c r="I8" s="3"/>
       <c r="J8" s="3"/>
     </row>
-    <row r="9" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>31</v>
+        <v>19</v>
       </c>
       <c r="B9">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>110</v>
+        <v>60</v>
       </c>
       <c r="D9" t="s">
-        <v>109</v>
+        <v>33</v>
       </c>
       <c r="E9" t="s">
-        <v>108</v>
+        <v>20</v>
       </c>
       <c r="F9" s="3">
-        <v>10</v>
-      </c>
-      <c r="G9" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="H9" s="3" t="s">
-        <v>112</v>
-      </c>
-      <c r="I9" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="J9" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="K9" s="1" t="s">
-        <v>111</v>
-      </c>
+        <v>6</v>
+      </c>
+      <c r="G9" s="3"/>
+      <c r="H9" s="3"/>
+      <c r="I9" s="3"/>
+      <c r="J9" s="3"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>6</v>
+        <v>20</v>
       </c>
       <c r="B10">
-        <v>2025</v>
+        <v>2023</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="D10" t="s">
-        <v>54</v>
+        <v>34</v>
       </c>
       <c r="E10" t="s">
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="F10" s="3">
         <v>9</v>
@@ -1037,59 +1029,48 @@
       <c r="I10" s="3"/>
       <c r="J10" s="3"/>
     </row>
-    <row r="11" spans="1:11" ht="90" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="B11">
-        <v>2023</v>
+        <v>2024</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>75</v>
+        <v>62</v>
       </c>
       <c r="D11" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="E11" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="F11" s="3">
-        <v>9</v>
-      </c>
-      <c r="G11" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="H11" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="I11" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="J11" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="K11" s="1" t="s">
-        <v>93</v>
-      </c>
+        <v>3</v>
+      </c>
+      <c r="G11" s="3"/>
+      <c r="H11" s="3"/>
+      <c r="I11" s="3"/>
+      <c r="J11" s="3"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="B12">
-        <v>2023</v>
+        <v>2024</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="D12" t="s">
-        <v>35</v>
+        <v>47</v>
       </c>
       <c r="E12" t="s">
-        <v>21</v>
+        <v>7</v>
       </c>
       <c r="F12" s="3">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="G12" s="3"/>
       <c r="H12" s="3"/>
@@ -1098,19 +1079,19 @@
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13">
-        <v>26</v>
+        <v>6</v>
       </c>
       <c r="B13">
-        <v>2014</v>
+        <v>2025</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>94</v>
+        <v>64</v>
       </c>
       <c r="D13" t="s">
-        <v>99</v>
+        <v>53</v>
       </c>
       <c r="E13" t="s">
-        <v>103</v>
+        <v>8</v>
       </c>
       <c r="F13" s="3">
         <v>9</v>
@@ -1122,22 +1103,22 @@
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14">
-        <v>27</v>
+        <v>7</v>
       </c>
       <c r="B14">
-        <v>2018</v>
+        <v>2023</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>95</v>
+        <v>65</v>
       </c>
       <c r="D14" t="s">
-        <v>100</v>
+        <v>46</v>
       </c>
       <c r="E14" t="s">
-        <v>105</v>
+        <v>9</v>
       </c>
       <c r="F14" s="3">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="G14" s="3"/>
       <c r="H14" s="3"/>
@@ -1146,22 +1127,22 @@
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="B15">
-        <v>2018</v>
+        <v>2019</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>97</v>
+        <v>66</v>
       </c>
       <c r="D15" t="s">
-        <v>100</v>
+        <v>32</v>
       </c>
       <c r="E15" t="s">
-        <v>106</v>
+        <v>19</v>
       </c>
       <c r="F15" s="3">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G15" s="3"/>
       <c r="H15" s="3"/>
@@ -1170,22 +1151,22 @@
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="B16">
-        <v>2022</v>
+        <v>2014</v>
       </c>
       <c r="C16" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="D16" t="s">
         <v>98</v>
       </c>
-      <c r="D16" t="s">
+      <c r="E16" t="s">
         <v>102</v>
       </c>
-      <c r="E16" t="s">
-        <v>107</v>
-      </c>
       <c r="F16" s="3">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G16" s="3"/>
       <c r="H16" s="3"/>
@@ -1194,153 +1175,155 @@
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17">
-        <v>1</v>
+        <v>30</v>
       </c>
       <c r="B17">
-        <v>2017</v>
+        <v>2022</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>82</v>
+        <v>97</v>
       </c>
       <c r="D17" t="s">
-        <v>43</v>
+        <v>101</v>
       </c>
       <c r="E17" t="s">
-        <v>58</v>
+        <v>106</v>
       </c>
       <c r="F17" s="3">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="G17" s="3"/>
       <c r="H17" s="3"/>
       <c r="I17" s="3"/>
       <c r="J17" s="3"/>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A18">
-        <v>3</v>
+        <v>31</v>
       </c>
       <c r="B18">
-        <v>2024</v>
+        <v>2022</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>59</v>
+        <v>109</v>
       </c>
       <c r="D18" t="s">
-        <v>42</v>
+        <v>108</v>
       </c>
       <c r="E18" t="s">
-        <v>5</v>
+        <v>107</v>
       </c>
       <c r="F18" s="3">
-        <v>7</v>
-      </c>
-      <c r="G18" s="3"/>
-      <c r="H18" s="3"/>
-      <c r="I18" s="3"/>
-      <c r="J18" s="3"/>
+        <v>10</v>
+      </c>
+      <c r="G18" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="H18" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="I18" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="J18" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="K18" s="1" t="s">
+        <v>110</v>
+      </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19">
+        <v>27</v>
+      </c>
+      <c r="B19">
+        <v>2018</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="D19" t="s">
+        <v>99</v>
+      </c>
+      <c r="E19" t="s">
+        <v>104</v>
+      </c>
+      <c r="F19" s="3">
         <v>8</v>
-      </c>
-      <c r="B19">
-        <v>2025</v>
-      </c>
-      <c r="C19" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="D19" t="s">
-        <v>44</v>
-      </c>
-      <c r="E19" t="s">
-        <v>92</v>
-      </c>
-      <c r="F19" s="3">
-        <v>7</v>
       </c>
       <c r="G19" s="3"/>
       <c r="H19" s="3"/>
       <c r="I19" s="3"/>
       <c r="J19" s="3"/>
     </row>
-    <row r="20" spans="1:11" ht="75" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20">
-        <v>11</v>
+        <v>29</v>
       </c>
       <c r="B20">
-        <v>2024</v>
+        <v>2018</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>83</v>
+        <v>96</v>
       </c>
       <c r="D20" t="s">
-        <v>45</v>
+        <v>99</v>
       </c>
       <c r="E20" t="s">
-        <v>12</v>
+        <v>105</v>
       </c>
       <c r="F20" s="3">
-        <v>7</v>
-      </c>
-      <c r="G20" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="H20" s="3" t="s">
-        <v>112</v>
-      </c>
-      <c r="I20" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="J20" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="K20" s="1" t="s">
-        <v>113</v>
-      </c>
+        <v>8</v>
+      </c>
+      <c r="G20" s="3"/>
+      <c r="H20" s="3"/>
+      <c r="I20" s="3"/>
+      <c r="J20" s="3"/>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21">
-        <v>17</v>
+        <v>28</v>
       </c>
       <c r="B21">
-        <v>2022</v>
+        <v>2021</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>70</v>
+        <v>95</v>
       </c>
       <c r="D21" t="s">
-        <v>31</v>
+        <v>100</v>
       </c>
       <c r="E21" t="s">
-        <v>18</v>
+        <v>103</v>
       </c>
       <c r="F21" s="3">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="G21" s="3"/>
       <c r="H21" s="3"/>
       <c r="I21" s="3"/>
-      <c r="J21" s="3"/>
+      <c r="J21" s="3" t="s">
+        <v>85</v>
+      </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B22">
         <v>2019</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D22" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="E22" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="F22" s="3">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="G22" s="3"/>
       <c r="H22" s="3"/>
@@ -1355,10 +1338,10 @@
         <v>2022</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D23" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E23" t="s">
         <v>24</v>
@@ -1373,22 +1356,22 @@
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="B24">
-        <v>2024</v>
+        <v>2022</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
       <c r="D24" t="s">
-        <v>48</v>
+        <v>31</v>
       </c>
       <c r="E24" t="s">
+        <v>18</v>
+      </c>
+      <c r="F24" s="3">
         <v>7</v>
-      </c>
-      <c r="F24" s="3">
-        <v>6</v>
       </c>
       <c r="G24" s="3"/>
       <c r="H24" s="3"/>
@@ -1397,43 +1380,43 @@
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="B25">
-        <v>2021</v>
+        <v>2025</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="D25" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="E25" t="s">
-        <v>14</v>
+        <v>91</v>
       </c>
       <c r="F25" s="3">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="G25" s="3"/>
       <c r="H25" s="3"/>
       <c r="I25" s="3"/>
       <c r="J25" s="3"/>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A26">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="B26">
-        <v>2023</v>
+        <v>2022</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="D26" t="s">
-        <v>56</v>
-      </c>
-      <c r="E26" t="s">
-        <v>16</v>
+        <v>35</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>22</v>
       </c>
       <c r="F26" s="3">
         <v>6</v>
@@ -1445,91 +1428,113 @@
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27">
-        <v>19</v>
+        <v>9</v>
       </c>
       <c r="B27">
         <v>2023</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>61</v>
+        <v>73</v>
       </c>
       <c r="D27" t="s">
-        <v>34</v>
+        <v>48</v>
       </c>
       <c r="E27" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="F27" s="3">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G27" s="3"/>
       <c r="H27" s="3"/>
       <c r="I27" s="3"/>
       <c r="J27" s="3"/>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11" ht="90" x14ac:dyDescent="0.25">
       <c r="A28">
-        <v>21</v>
+        <v>10</v>
       </c>
       <c r="B28">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="D28" t="s">
-        <v>36</v>
-      </c>
-      <c r="E28" s="1" t="s">
-        <v>22</v>
+        <v>54</v>
+      </c>
+      <c r="E28" t="s">
+        <v>11</v>
       </c>
       <c r="F28" s="3">
-        <v>6</v>
-      </c>
-      <c r="G28" s="3"/>
-      <c r="H28" s="3"/>
-      <c r="I28" s="3"/>
-      <c r="J28" s="3"/>
-    </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+      <c r="G28" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="H28" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="I28" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="J28" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="K28" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A29">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="B29">
-        <v>2025</v>
+        <v>2024</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>60</v>
+        <v>82</v>
       </c>
       <c r="D29" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="E29" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="F29" s="3">
-        <v>5</v>
-      </c>
-      <c r="G29" s="3"/>
-      <c r="H29" s="3"/>
-      <c r="I29" s="3"/>
-      <c r="J29" s="3"/>
+        <v>7</v>
+      </c>
+      <c r="G29" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="H29" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="I29" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="J29" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="K29" s="1" t="s">
+        <v>112</v>
+      </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30">
-        <v>7</v>
+        <v>24</v>
       </c>
       <c r="B30">
-        <v>2023</v>
+        <v>2024</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>66</v>
+        <v>75</v>
       </c>
       <c r="D30" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="E30" t="s">
-        <v>9</v>
+        <v>25</v>
       </c>
       <c r="F30" s="3">
         <v>5</v>
@@ -1541,19 +1546,19 @@
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="B31">
-        <v>2023</v>
+        <v>2024</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="D31" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="E31" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="F31" s="3">
         <v>5</v>
@@ -1565,22 +1570,22 @@
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32">
-        <v>12</v>
+        <v>22</v>
       </c>
       <c r="B32">
         <v>2024</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>77</v>
+        <v>67</v>
       </c>
       <c r="D32" t="s">
-        <v>51</v>
+        <v>37</v>
       </c>
       <c r="E32" t="s">
-        <v>13</v>
+        <v>23</v>
       </c>
       <c r="F32" s="3">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="G32" s="3"/>
       <c r="H32" s="3"/>
@@ -1589,22 +1594,22 @@
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B33">
-        <v>2019</v>
+        <v>2021</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>69</v>
+        <v>77</v>
       </c>
       <c r="D33" t="s">
-        <v>30</v>
+        <v>45</v>
       </c>
       <c r="E33" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="F33" s="3">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="G33" s="3"/>
       <c r="H33" s="3"/>
@@ -1613,22 +1618,22 @@
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B34">
         <v>2024</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="D34" t="s">
         <v>40</v>
       </c>
       <c r="E34" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="F34" s="3">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="G34" s="3"/>
       <c r="H34" s="3"/>
@@ -1643,10 +1648,10 @@
         <v>2023</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D35" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E35" t="s">
         <v>15</v>
@@ -1661,61 +1666,81 @@
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36">
-        <v>4</v>
+        <v>15</v>
       </c>
       <c r="B36">
-        <v>2024</v>
+        <v>2023</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>63</v>
+        <v>80</v>
       </c>
       <c r="D36" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="E36" t="s">
+        <v>16</v>
+      </c>
+      <c r="F36" s="3">
         <v>6</v>
-      </c>
-      <c r="F36" s="3">
-        <v>3</v>
       </c>
       <c r="G36" s="3"/>
       <c r="H36" s="3"/>
       <c r="I36" s="3"/>
       <c r="J36" s="3"/>
     </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>32</v>
+      </c>
+      <c r="B37">
+        <v>2018</v>
+      </c>
+      <c r="D37" t="s">
+        <v>114</v>
+      </c>
+      <c r="F37" s="3"/>
+      <c r="G37" s="3"/>
+      <c r="H37" s="3"/>
+      <c r="I37" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="J37" s="3" t="s">
+        <v>85</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C10" r:id="rId1" xr:uid="{662C990B-B86A-4079-894A-3E3E5E65D958}"/>
-    <hyperlink ref="C30" r:id="rId2" xr:uid="{6C418B6D-6C0C-43CB-9861-B0A9C3405037}"/>
-    <hyperlink ref="C25" r:id="rId3" xr:uid="{687D37D5-6A53-4809-B0D4-39187B9CDB51}"/>
+    <hyperlink ref="C13" r:id="rId1" xr:uid="{662C990B-B86A-4079-894A-3E3E5E65D958}"/>
+    <hyperlink ref="C14" r:id="rId2" xr:uid="{6C418B6D-6C0C-43CB-9861-B0A9C3405037}"/>
+    <hyperlink ref="C33" r:id="rId3" xr:uid="{687D37D5-6A53-4809-B0D4-39187B9CDB51}"/>
     <hyperlink ref="C35" r:id="rId4" xr:uid="{76EB6431-BC9E-4F14-A71B-C6B95C564741}"/>
-    <hyperlink ref="C26" r:id="rId5" xr:uid="{ED027085-A4A7-4B84-A093-30D4B8946EC5}"/>
-    <hyperlink ref="C22" r:id="rId6" xr:uid="{DE3AD58A-9EF7-4B73-9497-2A6221CBF2BA}"/>
-    <hyperlink ref="C27" r:id="rId7" xr:uid="{E87626ED-A48A-46C1-B0A1-D92709122E5D}"/>
-    <hyperlink ref="C28" r:id="rId8" xr:uid="{F18B3E29-0693-4E1D-A563-29F1B6D7D473}"/>
-    <hyperlink ref="C6" r:id="rId9" xr:uid="{FBA6D984-389D-4666-AF69-2DF781698029}"/>
-    <hyperlink ref="C7" r:id="rId10" xr:uid="{8419B468-9260-4EC4-B8B1-51A4A07F19E0}"/>
-    <hyperlink ref="C11" r:id="rId11" xr:uid="{7DF0F400-5600-4B7E-B147-67DA86069481}"/>
-    <hyperlink ref="C20" r:id="rId12" xr:uid="{2B967755-ACC4-42EE-98B5-27C84EBAFA42}"/>
-    <hyperlink ref="C32" r:id="rId13" xr:uid="{EE1231E6-9DB3-40E2-94A0-4ABC9DCA02F3}"/>
-    <hyperlink ref="C34" r:id="rId14" xr:uid="{94DF5807-DCFB-44C1-9A14-0E48C9156EC9}"/>
-    <hyperlink ref="C31" r:id="rId15" xr:uid="{FF7FB77C-809F-4107-A972-E7940B05389B}"/>
-    <hyperlink ref="C19" r:id="rId16" xr:uid="{DD854D55-9428-45F9-ACBC-BDC97A21F51F}"/>
-    <hyperlink ref="C21" r:id="rId17" xr:uid="{1F6B8341-332D-49CE-855C-75A637031AFC}"/>
+    <hyperlink ref="C36" r:id="rId5" xr:uid="{ED027085-A4A7-4B84-A093-30D4B8946EC5}"/>
+    <hyperlink ref="C15" r:id="rId6" xr:uid="{DE3AD58A-9EF7-4B73-9497-2A6221CBF2BA}"/>
+    <hyperlink ref="C9" r:id="rId7" xr:uid="{E87626ED-A48A-46C1-B0A1-D92709122E5D}"/>
+    <hyperlink ref="C26" r:id="rId8" xr:uid="{F18B3E29-0693-4E1D-A563-29F1B6D7D473}"/>
+    <hyperlink ref="C32" r:id="rId9" xr:uid="{FBA6D984-389D-4666-AF69-2DF781698029}"/>
+    <hyperlink ref="C34" r:id="rId10" xr:uid="{8419B468-9260-4EC4-B8B1-51A4A07F19E0}"/>
+    <hyperlink ref="C28" r:id="rId11" xr:uid="{7DF0F400-5600-4B7E-B147-67DA86069481}"/>
+    <hyperlink ref="C29" r:id="rId12" xr:uid="{2B967755-ACC4-42EE-98B5-27C84EBAFA42}"/>
+    <hyperlink ref="C31" r:id="rId13" xr:uid="{EE1231E6-9DB3-40E2-94A0-4ABC9DCA02F3}"/>
+    <hyperlink ref="C30" r:id="rId14" xr:uid="{94DF5807-DCFB-44C1-9A14-0E48C9156EC9}"/>
+    <hyperlink ref="C27" r:id="rId15" xr:uid="{FF7FB77C-809F-4107-A972-E7940B05389B}"/>
+    <hyperlink ref="C25" r:id="rId16" xr:uid="{DD854D55-9428-45F9-ACBC-BDC97A21F51F}"/>
+    <hyperlink ref="C24" r:id="rId17" xr:uid="{1F6B8341-332D-49CE-855C-75A637031AFC}"/>
     <hyperlink ref="C23" r:id="rId18" xr:uid="{3C15B722-4312-44AB-958D-DD3666D004AF}"/>
-    <hyperlink ref="C33" r:id="rId19" xr:uid="{61922079-14BC-47D8-82D1-7B7D9C9DE486}"/>
-    <hyperlink ref="C24" r:id="rId20" xr:uid="{503ADAC8-617F-48DD-8510-1FD61FF7DA22}"/>
-    <hyperlink ref="C36" r:id="rId21" xr:uid="{7001F43B-2968-46DB-AF8B-B7DD2691E5FD}"/>
-    <hyperlink ref="C12" r:id="rId22" xr:uid="{2DE5B6CE-7725-4C17-B5D4-0DFA9BD26432}"/>
-    <hyperlink ref="C18" r:id="rId23" xr:uid="{4944660B-A59A-41C2-9863-55EFDDE038AE}"/>
-    <hyperlink ref="C29" r:id="rId24" xr:uid="{C69B36F0-2B89-47B6-BC31-ACDF79F49B32}"/>
-    <hyperlink ref="C17" r:id="rId25" xr:uid="{03930357-F0F9-462D-A13B-CBD1C1B8C72E}"/>
-    <hyperlink ref="C13" r:id="rId26" xr:uid="{95A1E5A0-980E-4DB3-8046-566D2E946C8C}"/>
-    <hyperlink ref="C14" r:id="rId27" xr:uid="{7819739D-ADAC-426C-BC29-1A3209D63F34}"/>
-    <hyperlink ref="C8" r:id="rId28" xr:uid="{2D1D63DF-CA4E-4BC1-9C5C-6AF3A4C0CE05}"/>
-    <hyperlink ref="C15" r:id="rId29" xr:uid="{90402084-E9E4-4A3D-A1CA-D4B73CBB3CDE}"/>
-    <hyperlink ref="C16" r:id="rId30" xr:uid="{CB934A96-3CB2-4775-A540-BA09DC06EED6}"/>
-    <hyperlink ref="C9" r:id="rId31" xr:uid="{9E20CD7C-6E43-408A-93EB-504D56252D0E}"/>
+    <hyperlink ref="C22" r:id="rId19" xr:uid="{61922079-14BC-47D8-82D1-7B7D9C9DE486}"/>
+    <hyperlink ref="C12" r:id="rId20" xr:uid="{503ADAC8-617F-48DD-8510-1FD61FF7DA22}"/>
+    <hyperlink ref="C11" r:id="rId21" xr:uid="{7001F43B-2968-46DB-AF8B-B7DD2691E5FD}"/>
+    <hyperlink ref="C10" r:id="rId22" xr:uid="{2DE5B6CE-7725-4C17-B5D4-0DFA9BD26432}"/>
+    <hyperlink ref="C8" r:id="rId23" xr:uid="{4944660B-A59A-41C2-9863-55EFDDE038AE}"/>
+    <hyperlink ref="C7" r:id="rId24" xr:uid="{C69B36F0-2B89-47B6-BC31-ACDF79F49B32}"/>
+    <hyperlink ref="C6" r:id="rId25" xr:uid="{03930357-F0F9-462D-A13B-CBD1C1B8C72E}"/>
+    <hyperlink ref="C16" r:id="rId26" xr:uid="{95A1E5A0-980E-4DB3-8046-566D2E946C8C}"/>
+    <hyperlink ref="C19" r:id="rId27" xr:uid="{7819739D-ADAC-426C-BC29-1A3209D63F34}"/>
+    <hyperlink ref="C21" r:id="rId28" xr:uid="{2D1D63DF-CA4E-4BC1-9C5C-6AF3A4C0CE05}"/>
+    <hyperlink ref="C20" r:id="rId29" xr:uid="{90402084-E9E4-4A3D-A1CA-D4B73CBB3CDE}"/>
+    <hyperlink ref="C17" r:id="rId30" xr:uid="{CB934A96-3CB2-4775-A540-BA09DC06EED6}"/>
+    <hyperlink ref="C18" r:id="rId31" xr:uid="{9E20CD7C-6E43-408A-93EB-504D56252D0E}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">

</xml_diff>

<commit_message>
implementation of rating thresholds and other preprocessing techniques
</commit_message>
<xml_diff>
--- a/research papers/summary.xlsx
+++ b/research papers/summary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bradl\Desktop\uni\final-project\research papers\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{670AB422-E59F-47F1-8E04-5C1D2658E383}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{721CC8CB-42C2-4AA2-AFB2-C90B5FF73034}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="5280" windowWidth="29040" windowHeight="15840" xr2:uid="{85C2B9D3-E6D8-4805-9C5F-61C1282897A0}"/>
   </bookViews>
@@ -829,8 +829,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77C2DB88-371A-4ABD-A87E-357F7B7DC5EB}">
   <dimension ref="A1:K37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="D28" sqref="D28"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="E30" sqref="E30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>